<commit_message>
(#153)Refactored MegaMenu text length to be validated per sub menu
</commit_message>
<xml_diff>
--- a/test-data/mega-menu-data.xlsx
+++ b/test-data/mega-menu-data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashkinaea/IdeaProjects/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7651F5A4-CFF0-2F42-9A17-171C0EE3742B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C5F945-F815-AB4F-9B97-7912D5488A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4160" yWindow="-22080" windowWidth="31440" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33560" yWindow="2200" windowWidth="28800" windowHeight="16700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_menu" sheetId="1" r:id="rId1"/>
-    <sheet name="mega_menu_mobile" sheetId="4" r:id="rId2"/>
+    <sheet name="sub_menu" sheetId="5" r:id="rId2"/>
+    <sheet name="mega_menu_mobile" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>path</t>
   </si>
@@ -113,6 +114,21 @@
   </si>
   <si>
     <t>pediatric-adult-rare-tumor</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>boundary</t>
+  </si>
+  <si>
+    <t>250:500,250:500,350:550,400:600,150:350,200:400</t>
+  </si>
+  <si>
+    <t>250:450,250:450,250:450,50:150,120:320</t>
+  </si>
+  <si>
+    <t>espanol/cancer/sobrellevar/sentimientos</t>
   </si>
 </sst>
 </file>
@@ -487,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,6 +704,157 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132D59C2-63AE-5242-9460-21C6669FC236}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="87.1640625" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD69525-9B70-0B41-860F-5564C3609FDC}">
   <dimension ref="A1:B14"/>
   <sheetViews>

</xml_diff>